<commit_message>
Sprint 2 day 3 daily stadup
</commit_message>
<xml_diff>
--- a/Sprint_info/Sprint2.xlsx
+++ b/Sprint_info/Sprint2.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="56">
   <si>
     <t>Name</t>
   </si>
@@ -191,6 +191,12 @@
   </si>
   <si>
     <t>To do</t>
+  </si>
+  <si>
+    <t>In progress</t>
+  </si>
+  <si>
+    <t>Done</t>
   </si>
 </sst>
 </file>
@@ -380,24 +386,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -423,12 +411,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
@@ -440,6 +422,30 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="40% - Accent3" xfId="1" builtinId="39"/>
@@ -447,22 +453,7 @@
     <cellStyle name="Accent6" xfId="2" builtinId="49"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="7" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
+  <dxfs count="5">
     <dxf>
       <font>
         <color theme="0"/>
@@ -839,40 +830,40 @@
                   <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>37</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>37</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>37</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>37</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>37</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>37</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>37</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>37</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>37</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>37</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>37</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>37</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2107,21 +2098,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="12"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="24"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="7"/>
+      <c r="C2" s="19"/>
       <c r="D2" s="3" t="s">
         <v>2</v>
       </c>
@@ -2130,10 +2121,10 @@
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="8"/>
+      <c r="C3" s="20"/>
       <c r="D3" s="5" t="s">
         <v>8</v>
       </c>
@@ -2142,10 +2133,10 @@
       <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="8"/>
+      <c r="C4" s="20"/>
       <c r="D4" s="5" t="s">
         <v>5</v>
       </c>
@@ -2154,10 +2145,10 @@
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="9"/>
+      <c r="C5" s="21"/>
       <c r="D5" s="6" t="s">
         <v>11</v>
       </c>
@@ -2179,722 +2170,728 @@
   <dimension ref="A1:U24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" style="13" customWidth="1"/>
-    <col min="3" max="3" width="37.42578125" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14" style="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="15" width="5.7109375" style="13" customWidth="1"/>
-    <col min="16" max="19" width="6.7109375" style="13" customWidth="1"/>
-    <col min="20" max="20" width="6.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.42578125" style="13" bestFit="1" customWidth="1"/>
-    <col min="22" max="16384" width="9.140625" style="13"/>
+    <col min="1" max="1" width="19.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="37.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="15" width="5.7109375" style="7" customWidth="1"/>
+    <col min="16" max="19" width="6.7109375" style="7" customWidth="1"/>
+    <col min="20" max="20" width="6.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="15">
+      <c r="C1" s="9">
         <v>42449</v>
       </c>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="18">
+      <c r="C2" s="12">
         <f>C1+14</f>
         <v>42463</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="20" t="s">
+      <c r="D4" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="19" t="s">
+      <c r="E4" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="20" t="s">
+      <c r="F4" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="19" t="s">
+      <c r="G4" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="19" t="s">
+      <c r="H4" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="19" t="s">
+      <c r="I4" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="J4" s="19" t="s">
+      <c r="J4" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="K4" s="19" t="s">
+      <c r="K4" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="L4" s="19" t="s">
+      <c r="L4" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="M4" s="19" t="s">
+      <c r="M4" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="N4" s="19" t="s">
+      <c r="N4" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="O4" s="19" t="s">
+      <c r="O4" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="P4" s="19" t="s">
+      <c r="P4" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="Q4" s="19" t="s">
+      <c r="Q4" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="R4" s="19" t="s">
+      <c r="R4" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="S4" s="19" t="s">
+      <c r="S4" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="T4" s="19" t="s">
+      <c r="T4" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="U4" s="20" t="s">
+      <c r="U4" s="14" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="B5" s="22">
+      <c r="B5" s="25">
         <v>8</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="23">
+      <c r="E5" s="15">
         <v>3</v>
       </c>
-      <c r="F5" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="23"/>
-      <c r="J5" s="23"/>
-      <c r="K5" s="23"/>
-      <c r="L5" s="23"/>
-      <c r="M5" s="23"/>
-      <c r="N5" s="23"/>
-      <c r="O5" s="23"/>
-      <c r="P5" s="23"/>
-      <c r="Q5" s="23"/>
-      <c r="R5" s="23"/>
-      <c r="S5" s="23"/>
-      <c r="T5" s="23"/>
-      <c r="U5" s="23">
+      <c r="F5" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15">
+        <v>1</v>
+      </c>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="15"/>
+      <c r="P5" s="15"/>
+      <c r="Q5" s="15"/>
+      <c r="R5" s="15"/>
+      <c r="S5" s="15"/>
+      <c r="T5" s="15"/>
+      <c r="U5" s="15">
         <f>E5-SUM(G5:T5)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="22"/>
-      <c r="B6" s="22"/>
-      <c r="C6" s="23" t="s">
+      <c r="A6" s="25"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="D6" s="23" t="s">
+      <c r="D6" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="23">
+      <c r="E6" s="15">
         <v>5</v>
       </c>
-      <c r="F6" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="23"/>
-      <c r="J6" s="23"/>
-      <c r="K6" s="23"/>
-      <c r="L6" s="23"/>
-      <c r="M6" s="23"/>
-      <c r="N6" s="23"/>
-      <c r="O6" s="23"/>
-      <c r="P6" s="23"/>
-      <c r="Q6" s="23"/>
-      <c r="R6" s="23"/>
-      <c r="T6" s="23"/>
-      <c r="U6" s="23">
+      <c r="F6" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15">
+        <v>5</v>
+      </c>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="15"/>
+      <c r="P6" s="15"/>
+      <c r="Q6" s="15"/>
+      <c r="R6" s="15"/>
+      <c r="T6" s="15"/>
+      <c r="U6" s="15">
         <f t="shared" ref="U6:U16" si="0">E6-SUM(G6:T6)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7" s="22"/>
-      <c r="B7" s="22"/>
-      <c r="C7" s="23" t="s">
+      <c r="A7" s="25"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23">
+      <c r="D7" s="15"/>
+      <c r="E7" s="15">
         <v>1</v>
       </c>
-      <c r="F7" s="23" t="s">
+      <c r="F7" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="G7" s="23"/>
-      <c r="H7" s="23"/>
-      <c r="I7" s="23"/>
-      <c r="J7" s="23"/>
-      <c r="K7" s="23"/>
-      <c r="L7" s="23"/>
-      <c r="M7" s="23"/>
-      <c r="N7" s="23"/>
-      <c r="O7" s="23"/>
-      <c r="P7" s="23"/>
-      <c r="Q7" s="23"/>
-      <c r="R7" s="23"/>
-      <c r="S7" s="23"/>
-      <c r="T7" s="23"/>
-      <c r="U7" s="23">
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="15"/>
+      <c r="N7" s="15"/>
+      <c r="O7" s="15"/>
+      <c r="P7" s="15"/>
+      <c r="Q7" s="15"/>
+      <c r="R7" s="15"/>
+      <c r="S7" s="15"/>
+      <c r="T7" s="15"/>
+      <c r="U7" s="15">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="B8" s="22">
+      <c r="B8" s="25">
         <v>8</v>
       </c>
-      <c r="C8" s="23" t="s">
+      <c r="C8" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="D8" s="23" t="s">
+      <c r="D8" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E8" s="23">
+      <c r="E8" s="15">
         <v>3</v>
       </c>
-      <c r="F8" s="23" t="s">
+      <c r="F8" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="G8" s="23"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="23"/>
-      <c r="K8" s="23"/>
-      <c r="L8" s="23"/>
-      <c r="M8" s="23"/>
-      <c r="N8" s="23"/>
-      <c r="O8" s="23"/>
-      <c r="P8" s="23"/>
-      <c r="Q8" s="23"/>
-      <c r="R8" s="23"/>
-      <c r="S8" s="23"/>
-      <c r="T8" s="23"/>
-      <c r="U8" s="23">
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="15"/>
+      <c r="O8" s="15"/>
+      <c r="P8" s="15"/>
+      <c r="Q8" s="15"/>
+      <c r="R8" s="15"/>
+      <c r="S8" s="15"/>
+      <c r="T8" s="15"/>
+      <c r="U8" s="15">
         <f>E8-SUM(G8:T8)</f>
         <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A9" s="22"/>
-      <c r="B9" s="22"/>
-      <c r="C9" s="23" t="s">
+      <c r="A9" s="25"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23">
+      <c r="D9" s="15"/>
+      <c r="E9" s="15">
         <v>3</v>
       </c>
-      <c r="F9" s="23" t="s">
+      <c r="F9" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="G9" s="23"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="23"/>
-      <c r="J9" s="23"/>
-      <c r="K9" s="23"/>
-      <c r="L9" s="23"/>
-      <c r="M9" s="23"/>
-      <c r="N9" s="23"/>
-      <c r="O9" s="23"/>
-      <c r="P9" s="23"/>
-      <c r="Q9" s="23"/>
-      <c r="R9" s="23"/>
-      <c r="S9" s="23"/>
-      <c r="T9" s="23"/>
-      <c r="U9" s="23">
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="15"/>
+      <c r="O9" s="15"/>
+      <c r="P9" s="15"/>
+      <c r="Q9" s="15"/>
+      <c r="R9" s="15"/>
+      <c r="S9" s="15"/>
+      <c r="T9" s="15"/>
+      <c r="U9" s="15">
         <f t="shared" ref="U9:U10" si="1">E9-SUM(G9:T9)</f>
         <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="22"/>
-      <c r="B10" s="22"/>
-      <c r="C10" s="23" t="s">
+      <c r="A10" s="25"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23">
+      <c r="D10" s="15"/>
+      <c r="E10" s="15">
         <v>3</v>
       </c>
-      <c r="F10" s="23" t="s">
+      <c r="F10" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="G10" s="23"/>
-      <c r="H10" s="23"/>
-      <c r="I10" s="23"/>
-      <c r="J10" s="23"/>
-      <c r="K10" s="23"/>
-      <c r="L10" s="23"/>
-      <c r="M10" s="23"/>
-      <c r="N10" s="23"/>
-      <c r="O10" s="23"/>
-      <c r="P10" s="23"/>
-      <c r="Q10" s="23"/>
-      <c r="R10" s="23"/>
-      <c r="S10" s="23"/>
-      <c r="T10" s="23"/>
-      <c r="U10" s="23">
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15"/>
+      <c r="M10" s="15"/>
+      <c r="N10" s="15"/>
+      <c r="O10" s="15"/>
+      <c r="P10" s="15"/>
+      <c r="Q10" s="15"/>
+      <c r="R10" s="15"/>
+      <c r="S10" s="15"/>
+      <c r="T10" s="15"/>
+      <c r="U10" s="15">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="21" t="s">
+      <c r="A11" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="B11" s="22">
+      <c r="B11" s="25">
         <v>20</v>
       </c>
-      <c r="C11" s="23" t="s">
+      <c r="C11" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23">
+      <c r="D11" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="15">
         <v>5</v>
       </c>
-      <c r="F11" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="G11" s="23"/>
-      <c r="H11" s="23"/>
-      <c r="I11" s="23"/>
-      <c r="J11" s="23"/>
-      <c r="K11" s="23"/>
-      <c r="L11" s="23"/>
-      <c r="M11" s="23"/>
-      <c r="N11" s="23"/>
-      <c r="O11" s="23"/>
-      <c r="P11" s="23"/>
-      <c r="Q11" s="23"/>
-      <c r="R11" s="23"/>
-      <c r="S11" s="23"/>
-      <c r="T11" s="23"/>
-      <c r="U11" s="23">
+      <c r="F11" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="15"/>
+      <c r="N11" s="15"/>
+      <c r="O11" s="15"/>
+      <c r="P11" s="15"/>
+      <c r="Q11" s="15"/>
+      <c r="R11" s="15"/>
+      <c r="S11" s="15"/>
+      <c r="T11" s="15"/>
+      <c r="U11" s="15">
         <f>E11-SUM(G11:T11)</f>
         <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="21"/>
-      <c r="B12" s="22"/>
-      <c r="C12" s="23" t="s">
+      <c r="A12" s="26"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23">
+      <c r="D12" s="15"/>
+      <c r="E12" s="15">
         <v>5</v>
       </c>
-      <c r="F12" s="23" t="s">
+      <c r="F12" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="G12" s="23"/>
-      <c r="H12" s="23"/>
-      <c r="I12" s="23"/>
-      <c r="J12" s="23"/>
-      <c r="K12" s="23"/>
-      <c r="L12" s="23"/>
-      <c r="M12" s="23"/>
-      <c r="N12" s="23"/>
-      <c r="O12" s="23"/>
-      <c r="P12" s="23"/>
-      <c r="Q12" s="23"/>
-      <c r="R12" s="23"/>
-      <c r="S12" s="23"/>
-      <c r="T12" s="23"/>
-      <c r="U12" s="23">
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="15"/>
+      <c r="M12" s="15"/>
+      <c r="N12" s="15"/>
+      <c r="O12" s="15"/>
+      <c r="P12" s="15"/>
+      <c r="Q12" s="15"/>
+      <c r="R12" s="15"/>
+      <c r="S12" s="15"/>
+      <c r="T12" s="15"/>
+      <c r="U12" s="15">
         <f>E12-SUM(G12:T12)</f>
         <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="22"/>
-      <c r="B13" s="22"/>
-      <c r="C13" s="23" t="s">
+      <c r="A13" s="25"/>
+      <c r="B13" s="25"/>
+      <c r="C13" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="D13" s="23"/>
-      <c r="E13" s="23">
+      <c r="D13" s="15"/>
+      <c r="E13" s="15">
         <v>5</v>
       </c>
-      <c r="F13" s="23" t="s">
+      <c r="F13" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="G13" s="23"/>
-      <c r="H13" s="23"/>
-      <c r="I13" s="23"/>
-      <c r="J13" s="23"/>
-      <c r="K13" s="23"/>
-      <c r="L13" s="23"/>
-      <c r="M13" s="23"/>
-      <c r="N13" s="23"/>
-      <c r="O13" s="23"/>
-      <c r="P13" s="23"/>
-      <c r="Q13" s="23"/>
-      <c r="R13" s="23"/>
-      <c r="S13" s="23"/>
-      <c r="T13" s="23"/>
-      <c r="U13" s="23">
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="15"/>
+      <c r="N13" s="15"/>
+      <c r="O13" s="15"/>
+      <c r="P13" s="15"/>
+      <c r="Q13" s="15"/>
+      <c r="R13" s="15"/>
+      <c r="S13" s="15"/>
+      <c r="T13" s="15"/>
+      <c r="U13" s="15">
         <f t="shared" ref="U13:U15" si="2">E13-SUM(G13:T13)</f>
         <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="22"/>
-      <c r="B14" s="22"/>
-      <c r="C14" s="23" t="s">
+      <c r="A14" s="25"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="D14" s="23"/>
-      <c r="E14" s="23">
+      <c r="D14" s="15"/>
+      <c r="E14" s="15">
         <v>1</v>
       </c>
-      <c r="F14" s="23" t="s">
+      <c r="F14" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="G14" s="23"/>
-      <c r="H14" s="23"/>
-      <c r="I14" s="23"/>
-      <c r="J14" s="23"/>
-      <c r="K14" s="23"/>
-      <c r="L14" s="23"/>
-      <c r="M14" s="23"/>
-      <c r="N14" s="23"/>
-      <c r="O14" s="23"/>
-      <c r="P14" s="23"/>
-      <c r="Q14" s="23"/>
-      <c r="R14" s="23"/>
-      <c r="S14" s="23"/>
-      <c r="T14" s="23"/>
-      <c r="U14" s="23">
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="15"/>
+      <c r="M14" s="15"/>
+      <c r="N14" s="15"/>
+      <c r="O14" s="15"/>
+      <c r="P14" s="15"/>
+      <c r="Q14" s="15"/>
+      <c r="R14" s="15"/>
+      <c r="S14" s="15"/>
+      <c r="T14" s="15"/>
+      <c r="U14" s="15">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="22"/>
-      <c r="B15" s="22"/>
-      <c r="C15" s="23" t="s">
+      <c r="A15" s="25"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="D15" s="23"/>
-      <c r="E15" s="23">
+      <c r="D15" s="15"/>
+      <c r="E15" s="15">
         <v>3</v>
       </c>
-      <c r="F15" s="23" t="s">
+      <c r="F15" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="G15" s="23"/>
-      <c r="H15" s="23"/>
-      <c r="I15" s="23"/>
-      <c r="J15" s="23"/>
-      <c r="K15" s="23"/>
-      <c r="L15" s="23"/>
-      <c r="M15" s="23"/>
-      <c r="N15" s="23"/>
-      <c r="O15" s="23"/>
-      <c r="P15" s="23"/>
-      <c r="Q15" s="23"/>
-      <c r="R15" s="23"/>
-      <c r="S15" s="23"/>
-      <c r="T15" s="23"/>
-      <c r="U15" s="23">
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15"/>
+      <c r="L15" s="15"/>
+      <c r="M15" s="15"/>
+      <c r="N15" s="15"/>
+      <c r="O15" s="15"/>
+      <c r="P15" s="15"/>
+      <c r="Q15" s="15"/>
+      <c r="R15" s="15"/>
+      <c r="S15" s="15"/>
+      <c r="T15" s="15"/>
+      <c r="U15" s="15">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="23" t="s">
+      <c r="A16" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="23">
+      <c r="B16" s="15">
         <f>SUM(B5:B15)</f>
         <v>36</v>
       </c>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="23">
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="15">
         <f>SUM(E5:E15)</f>
         <v>37</v>
       </c>
-      <c r="F16" s="24"/>
-      <c r="G16" s="23">
-        <f>SUM(G5:G15)</f>
+      <c r="F16" s="16"/>
+      <c r="G16" s="15">
+        <f t="shared" ref="G16:T16" si="3">SUM(G5:G15)</f>
         <v>0</v>
       </c>
-      <c r="H16" s="23">
-        <f>SUM(H5:H15)</f>
+      <c r="H16" s="15">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I16" s="23">
-        <f>SUM(I5:I15)</f>
+      <c r="I16" s="15">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="J16" s="15">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J16" s="23">
-        <f>SUM(J5:J15)</f>
+      <c r="K16" s="15">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="K16" s="23">
-        <f>SUM(K5:K15)</f>
+      <c r="L16" s="15">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="L16" s="23">
-        <f>SUM(L5:L15)</f>
+      <c r="M16" s="15">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M16" s="23">
-        <f>SUM(M5:M15)</f>
+      <c r="N16" s="15">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N16" s="23">
-        <f>SUM(N5:N15)</f>
+      <c r="O16" s="15">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="O16" s="23">
-        <f>SUM(O5:O15)</f>
+      <c r="P16" s="15">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="P16" s="23">
-        <f>SUM(P5:P15)</f>
+      <c r="Q16" s="15">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="Q16" s="23">
-        <f>SUM(Q5:Q15)</f>
+      <c r="R16" s="15">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="R16" s="23">
-        <f>SUM(R5:R15)</f>
+      <c r="S16" s="15">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="S16" s="23">
-        <f>SUM(S5:S15)</f>
+      <c r="T16" s="15">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="T16" s="23">
-        <f>SUM(T5:T15)</f>
-        <v>0</v>
-      </c>
-      <c r="U16" s="23">
+      <c r="U16" s="15">
         <f t="shared" si="0"/>
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A17" s="25"/>
-      <c r="B17" s="25"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="23" t="s">
+      <c r="A17" s="17"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="F17" s="23">
+      <c r="F17" s="15">
         <f>SUM(E5:E15)</f>
         <v>37</v>
       </c>
-      <c r="G17" s="26">
+      <c r="G17" s="18">
         <f>F17-F17/14</f>
         <v>34.357142857142854</v>
       </c>
-      <c r="H17" s="26">
+      <c r="H17" s="18">
         <f>G17-F17/14</f>
         <v>31.714285714285712</v>
       </c>
-      <c r="I17" s="26">
+      <c r="I17" s="18">
         <f>H17-F17/14</f>
         <v>29.071428571428569</v>
       </c>
-      <c r="J17" s="26">
+      <c r="J17" s="18">
         <f>I17-F17/14</f>
         <v>26.428571428571427</v>
       </c>
-      <c r="K17" s="26">
+      <c r="K17" s="18">
         <f>J17-F17/14</f>
         <v>23.785714285714285</v>
       </c>
-      <c r="L17" s="26">
+      <c r="L17" s="18">
         <f>K17-F17/14</f>
         <v>21.142857142857142</v>
       </c>
-      <c r="M17" s="26">
+      <c r="M17" s="18">
         <f>L17-F17/14</f>
         <v>18.5</v>
       </c>
-      <c r="N17" s="26">
+      <c r="N17" s="18">
         <f>M17-F17/14</f>
         <v>15.857142857142858</v>
       </c>
-      <c r="O17" s="26">
+      <c r="O17" s="18">
         <f>N17-F17/14</f>
         <v>13.214285714285715</v>
       </c>
-      <c r="P17" s="26">
+      <c r="P17" s="18">
         <f>O17-F17/14</f>
         <v>10.571428571428573</v>
       </c>
-      <c r="Q17" s="26">
+      <c r="Q17" s="18">
         <f>P17-F17/14</f>
         <v>7.9285714285714306</v>
       </c>
-      <c r="R17" s="26">
+      <c r="R17" s="18">
         <f>Q17-F17/14</f>
         <v>5.2857142857142883</v>
       </c>
-      <c r="S17" s="26">
+      <c r="S17" s="18">
         <f>R17-F17/14</f>
         <v>2.6428571428571455</v>
       </c>
-      <c r="T17" s="26">
+      <c r="T17" s="18">
         <f>S17-F17/14</f>
         <v>0</v>
       </c>
-      <c r="U17" s="25"/>
+      <c r="U17" s="17"/>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A18" s="25"/>
-      <c r="B18" s="25"/>
-      <c r="C18" s="25"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="23" t="s">
+      <c r="A18" s="17"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="F18" s="23">
+      <c r="F18" s="15">
         <f>SUM(E5:E15)</f>
         <v>37</v>
       </c>
-      <c r="G18" s="23">
-        <f>F18-SUM(G5:G15)</f>
+      <c r="G18" s="15">
+        <f t="shared" ref="G18:T18" si="4">F18-SUM(G5:G15)</f>
         <v>37</v>
       </c>
-      <c r="H18" s="23">
-        <f>G18-SUM(H5:H15)</f>
+      <c r="H18" s="15">
+        <f t="shared" si="4"/>
         <v>37</v>
       </c>
-      <c r="I18" s="23">
-        <f>H18-SUM(I5:I15)</f>
-        <v>37</v>
-      </c>
-      <c r="J18" s="23">
-        <f>I18-SUM(J5:J15)</f>
-        <v>37</v>
-      </c>
-      <c r="K18" s="23">
-        <f>J18-SUM(K5:K15)</f>
-        <v>37</v>
-      </c>
-      <c r="L18" s="23">
-        <f>K18-SUM(L5:L15)</f>
-        <v>37</v>
-      </c>
-      <c r="M18" s="23">
-        <f>L18-SUM(M5:M15)</f>
-        <v>37</v>
-      </c>
-      <c r="N18" s="23">
-        <f>M18-SUM(N5:N15)</f>
-        <v>37</v>
-      </c>
-      <c r="O18" s="23">
-        <f>N18-SUM(O5:O15)</f>
-        <v>37</v>
-      </c>
-      <c r="P18" s="23">
-        <f>O18-SUM(P5:P15)</f>
-        <v>37</v>
-      </c>
-      <c r="Q18" s="23">
-        <f>P18-SUM(Q5:Q15)</f>
-        <v>37</v>
-      </c>
-      <c r="R18" s="23">
-        <f>Q18-SUM(R5:R15)</f>
-        <v>37</v>
-      </c>
-      <c r="S18" s="23">
-        <f>R18-SUM(S5:S15)</f>
-        <v>37</v>
-      </c>
-      <c r="T18" s="23">
-        <f>S18-SUM(T5:T15)</f>
-        <v>37</v>
-      </c>
-      <c r="U18" s="25"/>
+      <c r="I18" s="15">
+        <f t="shared" si="4"/>
+        <v>31</v>
+      </c>
+      <c r="J18" s="15">
+        <f t="shared" si="4"/>
+        <v>31</v>
+      </c>
+      <c r="K18" s="15">
+        <f t="shared" si="4"/>
+        <v>31</v>
+      </c>
+      <c r="L18" s="15">
+        <f t="shared" si="4"/>
+        <v>31</v>
+      </c>
+      <c r="M18" s="15">
+        <f t="shared" si="4"/>
+        <v>31</v>
+      </c>
+      <c r="N18" s="15">
+        <f t="shared" si="4"/>
+        <v>31</v>
+      </c>
+      <c r="O18" s="15">
+        <f t="shared" si="4"/>
+        <v>31</v>
+      </c>
+      <c r="P18" s="15">
+        <f t="shared" si="4"/>
+        <v>31</v>
+      </c>
+      <c r="Q18" s="15">
+        <f t="shared" si="4"/>
+        <v>31</v>
+      </c>
+      <c r="R18" s="15">
+        <f t="shared" si="4"/>
+        <v>31</v>
+      </c>
+      <c r="S18" s="15">
+        <f t="shared" si="4"/>
+        <v>31</v>
+      </c>
+      <c r="T18" s="15">
+        <f t="shared" si="4"/>
+        <v>31</v>
+      </c>
+      <c r="U18" s="17"/>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A20" s="25"/>
-      <c r="B20" s="25"/>
-      <c r="C20" s="25"/>
-      <c r="D20" s="25"/>
+      <c r="A20" s="17"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A21" s="25"/>
-      <c r="B21" s="25"/>
-      <c r="C21" s="25"/>
-      <c r="D21" s="25"/>
+      <c r="A21" s="17"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A22" s="25"/>
-      <c r="B22" s="25"/>
-      <c r="C22" s="25"/>
-      <c r="D22" s="25"/>
+      <c r="A22" s="17"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A23" s="25"/>
-      <c r="B23" s="25"/>
-      <c r="C23" s="25"/>
-      <c r="D23" s="25"/>
+      <c r="A23" s="17"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A24" s="25"/>
-      <c r="B24" s="25"/>
-      <c r="C24" s="25"/>
-      <c r="D24" s="25"/>
+      <c r="A24" s="17"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -2906,23 +2903,23 @@
     <mergeCell ref="B11:B15"/>
   </mergeCells>
   <conditionalFormatting sqref="F5:F15">
-    <cfRule type="cellIs" dxfId="7" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="11" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="13" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="14" operator="equal">
       <formula>"To do"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U5:U7 U11:U16">
-    <cfRule type="cellIs" dxfId="4" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="9" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U8:U10">
-    <cfRule type="cellIs" dxfId="3" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="5" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Sprint 2 daily standup day 6
</commit_message>
<xml_diff>
--- a/Sprint_info/Sprint2.xlsx
+++ b/Sprint_info/Sprint2.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="57">
   <si>
     <t>Name</t>
   </si>
@@ -197,6 +197,9 @@
   </si>
   <si>
     <t>Done</t>
+  </si>
+  <si>
+    <t>Review code</t>
   </si>
 </sst>
 </file>
@@ -594,7 +597,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sprint!$E$17</c:f>
+              <c:f>Sprint!$E$18</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -673,54 +676,54 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sprint!$F$17:$T$17</c:f>
+              <c:f>Sprint!$F$18:$T$18</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>37</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>34.357142857142854</c:v>
+                  <c:v>35.285714285714285</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>31.714285714285712</c:v>
+                  <c:v>32.571428571428569</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>29.071428571428569</c:v>
+                  <c:v>29.857142857142854</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>26.428571428571427</c:v>
+                  <c:v>27.142857142857139</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>23.785714285714285</c:v>
+                  <c:v>24.428571428571423</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>21.142857142857142</c:v>
+                  <c:v>21.714285714285708</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>18.5</c:v>
+                  <c:v>18.999999999999993</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>15.857142857142858</c:v>
+                  <c:v>16.285714285714278</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>13.214285714285715</c:v>
+                  <c:v>13.571428571428562</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10.571428571428573</c:v>
+                  <c:v>10.857142857142847</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>7.9285714285714306</c:v>
+                  <c:v>8.1428571428571317</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>5.2857142857142883</c:v>
+                  <c:v>5.4285714285714173</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.6428571428571455</c:v>
+                  <c:v>2.7142857142857029</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>-1.1546319456101628E-14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -737,7 +740,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sprint!$E$18</c:f>
+              <c:f>Sprint!$E$19</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -816,54 +819,54 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sprint!$F$18:$T$18</c:f>
+              <c:f>Sprint!$F$19:$T$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>37</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>37</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>37</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>31</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>31</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>31</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>31</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>31</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>31</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>31</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>31</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>31</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>31</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>31</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>31</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2167,10 +2170,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U24"/>
+  <dimension ref="A1:U25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2289,7 +2292,7 @@
         <v>3</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G5" s="15"/>
       <c r="H5" s="15"/>
@@ -2298,7 +2301,9 @@
       </c>
       <c r="J5" s="15"/>
       <c r="K5" s="15"/>
-      <c r="L5" s="15"/>
+      <c r="L5" s="15">
+        <v>2</v>
+      </c>
       <c r="M5" s="15"/>
       <c r="N5" s="15"/>
       <c r="O5" s="15"/>
@@ -2309,7 +2314,7 @@
       <c r="T5" s="15"/>
       <c r="U5" s="15">
         <f>E5-SUM(G5:T5)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
@@ -2343,7 +2348,7 @@
       <c r="R6" s="15"/>
       <c r="T6" s="15"/>
       <c r="U6" s="15">
-        <f t="shared" ref="U6:U16" si="0">E6-SUM(G6:T6)</f>
+        <f t="shared" ref="U6:U17" si="0">E6-SUM(G6:T6)</f>
         <v>0</v>
       </c>
     </row>
@@ -2455,7 +2460,9 @@
       <c r="C10" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="D10" s="15"/>
+      <c r="D10" s="15" t="s">
+        <v>9</v>
+      </c>
       <c r="E10" s="15">
         <v>3</v>
       </c>
@@ -2505,7 +2512,9 @@
       <c r="I11" s="15"/>
       <c r="J11" s="15"/>
       <c r="K11" s="15"/>
-      <c r="L11" s="15"/>
+      <c r="L11" s="15">
+        <v>1</v>
+      </c>
       <c r="M11" s="15"/>
       <c r="N11" s="15"/>
       <c r="O11" s="15"/>
@@ -2516,7 +2525,7 @@
       <c r="T11" s="15"/>
       <c r="U11" s="15">
         <f>E11-SUM(G11:T11)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2525,7 +2534,9 @@
       <c r="C12" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="D12" s="15"/>
+      <c r="D12" s="15" t="s">
+        <v>3</v>
+      </c>
       <c r="E12" s="15">
         <v>5</v>
       </c>
@@ -2579,7 +2590,7 @@
       <c r="S13" s="15"/>
       <c r="T13" s="15"/>
       <c r="U13" s="15">
-        <f t="shared" ref="U13:U15" si="2">E13-SUM(G13:T13)</f>
+        <f t="shared" ref="U13:U16" si="2">E13-SUM(G13:T13)</f>
         <v>5</v>
       </c>
     </row>
@@ -2589,7 +2600,9 @@
       <c r="C14" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="D14" s="15"/>
+      <c r="D14" s="15" t="s">
+        <v>6</v>
+      </c>
       <c r="E14" s="15">
         <v>1</v>
       </c>
@@ -2619,11 +2632,11 @@
       <c r="A15" s="25"/>
       <c r="B15" s="25"/>
       <c r="C15" s="15" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="D15" s="15"/>
       <c r="E15" s="15">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F15" s="15" t="s">
         <v>53</v>
@@ -2644,154 +2657,116 @@
       <c r="T15" s="15"/>
       <c r="U15" s="15">
         <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="25"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="B16" s="15">
-        <f>SUM(B5:B15)</f>
-        <v>36</v>
-      </c>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="15">
-        <f>SUM(E5:E15)</f>
-        <v>37</v>
-      </c>
-      <c r="F16" s="16"/>
-      <c r="G16" s="15">
-        <f t="shared" ref="G16:T16" si="3">SUM(G5:G15)</f>
-        <v>0</v>
-      </c>
-      <c r="H16" s="15">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="I16" s="15">
-        <f t="shared" si="3"/>
-        <v>6</v>
-      </c>
-      <c r="J16" s="15">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="K16" s="15">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L16" s="15">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="M16" s="15">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="N16" s="15">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="O16" s="15">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="P16" s="15">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="Q16" s="15">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="R16" s="15">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="S16" s="15">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="T16" s="15">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
+      <c r="F16" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="15"/>
+      <c r="L16" s="15"/>
+      <c r="M16" s="15"/>
+      <c r="N16" s="15"/>
+      <c r="O16" s="15"/>
+      <c r="P16" s="15"/>
+      <c r="Q16" s="15"/>
+      <c r="R16" s="15"/>
+      <c r="S16" s="15"/>
+      <c r="T16" s="15"/>
       <c r="U16" s="15">
-        <f t="shared" si="0"/>
-        <v>31</v>
+        <f t="shared" si="2"/>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A17" s="17"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="15" t="s">
+      <c r="A17" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" s="15">
+        <f>SUM(B5:B16)</f>
         <v>36</v>
       </c>
-      <c r="F17" s="15">
-        <f>SUM(E5:E15)</f>
-        <v>37</v>
-      </c>
-      <c r="G17" s="18">
-        <f>F17-F17/14</f>
-        <v>34.357142857142854</v>
-      </c>
-      <c r="H17" s="18">
-        <f>G17-F17/14</f>
-        <v>31.714285714285712</v>
-      </c>
-      <c r="I17" s="18">
-        <f>H17-F17/14</f>
-        <v>29.071428571428569</v>
-      </c>
-      <c r="J17" s="18">
-        <f>I17-F17/14</f>
-        <v>26.428571428571427</v>
-      </c>
-      <c r="K17" s="18">
-        <f>J17-F17/14</f>
-        <v>23.785714285714285</v>
-      </c>
-      <c r="L17" s="18">
-        <f>K17-F17/14</f>
-        <v>21.142857142857142</v>
-      </c>
-      <c r="M17" s="18">
-        <f>L17-F17/14</f>
-        <v>18.5</v>
-      </c>
-      <c r="N17" s="18">
-        <f>M17-F17/14</f>
-        <v>15.857142857142858</v>
-      </c>
-      <c r="O17" s="18">
-        <f>N17-F17/14</f>
-        <v>13.214285714285715</v>
-      </c>
-      <c r="P17" s="18">
-        <f>O17-F17/14</f>
-        <v>10.571428571428573</v>
-      </c>
-      <c r="Q17" s="18">
-        <f>P17-F17/14</f>
-        <v>7.9285714285714306</v>
-      </c>
-      <c r="R17" s="18">
-        <f>Q17-F17/14</f>
-        <v>5.2857142857142883</v>
-      </c>
-      <c r="S17" s="18">
-        <f>R17-F17/14</f>
-        <v>2.6428571428571455</v>
-      </c>
-      <c r="T17" s="18">
-        <f>S17-F17/14</f>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="15">
+        <f>SUM(E5:E16)</f>
+        <v>38</v>
+      </c>
+      <c r="F17" s="16"/>
+      <c r="G17" s="15">
+        <f>SUM(G5:G16)</f>
         <v>0</v>
       </c>
-      <c r="U17" s="17"/>
+      <c r="H17" s="15">
+        <f>SUM(H5:H16)</f>
+        <v>0</v>
+      </c>
+      <c r="I17" s="15">
+        <f>SUM(I5:I16)</f>
+        <v>6</v>
+      </c>
+      <c r="J17" s="15">
+        <f>SUM(J5:J16)</f>
+        <v>0</v>
+      </c>
+      <c r="K17" s="15">
+        <f>SUM(K5:K16)</f>
+        <v>0</v>
+      </c>
+      <c r="L17" s="15">
+        <f>SUM(L5:L16)</f>
+        <v>3</v>
+      </c>
+      <c r="M17" s="15">
+        <f>SUM(M5:M16)</f>
+        <v>0</v>
+      </c>
+      <c r="N17" s="15">
+        <f>SUM(N5:N16)</f>
+        <v>0</v>
+      </c>
+      <c r="O17" s="15">
+        <f>SUM(O5:O16)</f>
+        <v>0</v>
+      </c>
+      <c r="P17" s="15">
+        <f>SUM(P5:P16)</f>
+        <v>0</v>
+      </c>
+      <c r="Q17" s="15">
+        <f>SUM(Q5:Q16)</f>
+        <v>0</v>
+      </c>
+      <c r="R17" s="15">
+        <f>SUM(R5:R16)</f>
+        <v>0</v>
+      </c>
+      <c r="S17" s="15">
+        <f>SUM(S5:S16)</f>
+        <v>0</v>
+      </c>
+      <c r="T17" s="15">
+        <f>SUM(T5:T16)</f>
+        <v>0</v>
+      </c>
+      <c r="U17" s="15">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="17"/>
@@ -2799,75 +2774,139 @@
       <c r="C18" s="17"/>
       <c r="D18" s="17"/>
       <c r="E18" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F18" s="15">
-        <f>SUM(E5:E15)</f>
-        <v>37</v>
-      </c>
-      <c r="G18" s="15">
-        <f t="shared" ref="G18:T18" si="4">F18-SUM(G5:G15)</f>
-        <v>37</v>
-      </c>
-      <c r="H18" s="15">
-        <f t="shared" si="4"/>
-        <v>37</v>
-      </c>
-      <c r="I18" s="15">
-        <f t="shared" si="4"/>
-        <v>31</v>
-      </c>
-      <c r="J18" s="15">
-        <f t="shared" si="4"/>
-        <v>31</v>
-      </c>
-      <c r="K18" s="15">
-        <f t="shared" si="4"/>
-        <v>31</v>
-      </c>
-      <c r="L18" s="15">
-        <f t="shared" si="4"/>
-        <v>31</v>
-      </c>
-      <c r="M18" s="15">
-        <f t="shared" si="4"/>
-        <v>31</v>
-      </c>
-      <c r="N18" s="15">
-        <f t="shared" si="4"/>
-        <v>31</v>
-      </c>
-      <c r="O18" s="15">
-        <f t="shared" si="4"/>
-        <v>31</v>
-      </c>
-      <c r="P18" s="15">
-        <f t="shared" si="4"/>
-        <v>31</v>
-      </c>
-      <c r="Q18" s="15">
-        <f t="shared" si="4"/>
-        <v>31</v>
-      </c>
-      <c r="R18" s="15">
-        <f t="shared" si="4"/>
-        <v>31</v>
-      </c>
-      <c r="S18" s="15">
-        <f t="shared" si="4"/>
-        <v>31</v>
-      </c>
-      <c r="T18" s="15">
-        <f t="shared" si="4"/>
-        <v>31</v>
+        <f>SUM(E5:E16)</f>
+        <v>38</v>
+      </c>
+      <c r="G18" s="18">
+        <f>F18-F18/14</f>
+        <v>35.285714285714285</v>
+      </c>
+      <c r="H18" s="18">
+        <f>G18-F18/14</f>
+        <v>32.571428571428569</v>
+      </c>
+      <c r="I18" s="18">
+        <f>H18-F18/14</f>
+        <v>29.857142857142854</v>
+      </c>
+      <c r="J18" s="18">
+        <f>I18-F18/14</f>
+        <v>27.142857142857139</v>
+      </c>
+      <c r="K18" s="18">
+        <f>J18-F18/14</f>
+        <v>24.428571428571423</v>
+      </c>
+      <c r="L18" s="18">
+        <f>K18-F18/14</f>
+        <v>21.714285714285708</v>
+      </c>
+      <c r="M18" s="18">
+        <f>L18-F18/14</f>
+        <v>18.999999999999993</v>
+      </c>
+      <c r="N18" s="18">
+        <f>M18-F18/14</f>
+        <v>16.285714285714278</v>
+      </c>
+      <c r="O18" s="18">
+        <f>N18-F18/14</f>
+        <v>13.571428571428562</v>
+      </c>
+      <c r="P18" s="18">
+        <f>O18-F18/14</f>
+        <v>10.857142857142847</v>
+      </c>
+      <c r="Q18" s="18">
+        <f>P18-F18/14</f>
+        <v>8.1428571428571317</v>
+      </c>
+      <c r="R18" s="18">
+        <f>Q18-F18/14</f>
+        <v>5.4285714285714173</v>
+      </c>
+      <c r="S18" s="18">
+        <f>R18-F18/14</f>
+        <v>2.7142857142857029</v>
+      </c>
+      <c r="T18" s="18">
+        <f>S18-F18/14</f>
+        <v>-1.1546319456101628E-14</v>
       </c>
       <c r="U18" s="17"/>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A20" s="17"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A19" s="17"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F19" s="15">
+        <f>SUM(E5:E16)</f>
+        <v>38</v>
+      </c>
+      <c r="G19" s="15">
+        <f>F19-SUM(G5:G16)</f>
+        <v>38</v>
+      </c>
+      <c r="H19" s="15">
+        <f>G19-SUM(H5:H16)</f>
+        <v>38</v>
+      </c>
+      <c r="I19" s="15">
+        <f>H19-SUM(I5:I16)</f>
+        <v>32</v>
+      </c>
+      <c r="J19" s="15">
+        <f>I19-SUM(J5:J16)</f>
+        <v>32</v>
+      </c>
+      <c r="K19" s="15">
+        <f>J19-SUM(K5:K16)</f>
+        <v>32</v>
+      </c>
+      <c r="L19" s="15">
+        <f>K19-SUM(L5:L16)</f>
+        <v>29</v>
+      </c>
+      <c r="M19" s="15">
+        <f>L19-SUM(M5:M16)</f>
+        <v>29</v>
+      </c>
+      <c r="N19" s="15">
+        <f>M19-SUM(N5:N16)</f>
+        <v>29</v>
+      </c>
+      <c r="O19" s="15">
+        <f>N19-SUM(O5:O16)</f>
+        <v>29</v>
+      </c>
+      <c r="P19" s="15">
+        <f>O19-SUM(P5:P16)</f>
+        <v>29</v>
+      </c>
+      <c r="Q19" s="15">
+        <f>P19-SUM(Q5:Q16)</f>
+        <v>29</v>
+      </c>
+      <c r="R19" s="15">
+        <f>Q19-SUM(R5:R16)</f>
+        <v>29</v>
+      </c>
+      <c r="S19" s="15">
+        <f>R19-SUM(S5:S16)</f>
+        <v>29</v>
+      </c>
+      <c r="T19" s="15">
+        <f>S19-SUM(T5:T16)</f>
+        <v>29</v>
+      </c>
+      <c r="U19" s="17"/>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="17"/>
@@ -2893,16 +2932,22 @@
       <c r="C24" s="17"/>
       <c r="D24" s="17"/>
     </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A25" s="17"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="17"/>
+    </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="B5:B7"/>
     <mergeCell ref="A5:A7"/>
     <mergeCell ref="A8:A10"/>
     <mergeCell ref="B8:B10"/>
-    <mergeCell ref="A11:A15"/>
-    <mergeCell ref="B11:B15"/>
+    <mergeCell ref="A11:A16"/>
+    <mergeCell ref="B11:B16"/>
   </mergeCells>
-  <conditionalFormatting sqref="F5:F15">
+  <conditionalFormatting sqref="F5:F16">
     <cfRule type="cellIs" dxfId="4" priority="11" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
@@ -2913,7 +2958,7 @@
       <formula>"To do"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U5:U7 U11:U16">
+  <conditionalFormatting sqref="U5:U7 U11:U17">
     <cfRule type="cellIs" dxfId="1" priority="9" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
@@ -2924,7 +2969,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations xWindow="491" yWindow="329" count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F15">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F16">
       <formula1>"To do, In progress, Done"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2937,7 +2982,7 @@
           <x14:formula1>
             <xm:f>Roster!$A$3:$A$5</xm:f>
           </x14:formula1>
-          <xm:sqref>D5:D15</xm:sqref>
+          <xm:sqref>D5:D16</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Commited logo and documentation template
</commit_message>
<xml_diff>
--- a/Sprint_info/Sprint2.xlsx
+++ b/Sprint_info/Sprint2.xlsx
@@ -162,9 +162,6 @@
 for proffesor</t>
   </si>
   <si>
-    <t>Description project documentation</t>
-  </si>
-  <si>
     <t>Requirements documentation</t>
   </si>
   <si>
@@ -200,6 +197,9 @@
   </si>
   <si>
     <t>Review code</t>
+  </si>
+  <si>
+    <t>Project description documentation</t>
   </si>
 </sst>
 </file>
@@ -845,28 +845,28 @@
                   <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>29</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>29</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>29</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>29</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>29</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>29</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>29</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>29</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2173,7 +2173,7 @@
   <dimension ref="A1:U25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2292,7 +2292,7 @@
         <v>3</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G5" s="15"/>
       <c r="H5" s="15"/>
@@ -2330,7 +2330,7 @@
         <v>5</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G6" s="15"/>
       <c r="H6" s="15"/>
@@ -2363,7 +2363,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G7" s="15"/>
       <c r="H7" s="15"/>
@@ -2392,7 +2392,7 @@
         <v>8</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="D8" s="15" t="s">
         <v>3</v>
@@ -2426,14 +2426,14 @@
       <c r="A9" s="25"/>
       <c r="B9" s="25"/>
       <c r="C9" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D9" s="15"/>
       <c r="E9" s="15">
         <v>3</v>
       </c>
       <c r="F9" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G9" s="15"/>
       <c r="H9" s="15"/>
@@ -2458,7 +2458,7 @@
       <c r="A10" s="25"/>
       <c r="B10" s="25"/>
       <c r="C10" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D10" s="15" t="s">
         <v>9</v>
@@ -2467,7 +2467,7 @@
         <v>3</v>
       </c>
       <c r="F10" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G10" s="15"/>
       <c r="H10" s="15"/>
@@ -2490,13 +2490,13 @@
     </row>
     <row r="11" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="26" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B11" s="25">
         <v>20</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D11" s="15" t="s">
         <v>6</v>
@@ -2505,7 +2505,7 @@
         <v>5</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G11" s="15"/>
       <c r="H11" s="15"/>
@@ -2515,7 +2515,9 @@
       <c r="L11" s="15">
         <v>1</v>
       </c>
-      <c r="M11" s="15"/>
+      <c r="M11" s="15">
+        <v>3</v>
+      </c>
       <c r="N11" s="15"/>
       <c r="O11" s="15"/>
       <c r="P11" s="15"/>
@@ -2525,14 +2527,14 @@
       <c r="T11" s="15"/>
       <c r="U11" s="15">
         <f>E11-SUM(G11:T11)</f>
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="26"/>
       <c r="B12" s="25"/>
       <c r="C12" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D12" s="15" t="s">
         <v>3</v>
@@ -2541,7 +2543,7 @@
         <v>5</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G12" s="15"/>
       <c r="H12" s="15"/>
@@ -2566,14 +2568,14 @@
       <c r="A13" s="25"/>
       <c r="B13" s="25"/>
       <c r="C13" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D13" s="15"/>
       <c r="E13" s="15">
         <v>5</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G13" s="15"/>
       <c r="H13" s="15"/>
@@ -2598,7 +2600,7 @@
       <c r="A14" s="25"/>
       <c r="B14" s="25"/>
       <c r="C14" s="15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D14" s="15" t="s">
         <v>6</v>
@@ -2607,7 +2609,7 @@
         <v>1</v>
       </c>
       <c r="F14" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G14" s="15"/>
       <c r="H14" s="15"/>
@@ -2632,14 +2634,14 @@
       <c r="A15" s="25"/>
       <c r="B15" s="25"/>
       <c r="C15" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D15" s="15"/>
       <c r="E15" s="15">
         <v>1</v>
       </c>
       <c r="F15" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G15" s="15"/>
       <c r="H15" s="15"/>
@@ -2664,14 +2666,14 @@
       <c r="A16" s="25"/>
       <c r="B16" s="25"/>
       <c r="C16" s="15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D16" s="15"/>
       <c r="E16" s="15">
         <v>3</v>
       </c>
       <c r="F16" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G16" s="15"/>
       <c r="H16" s="15"/>
@@ -2708,64 +2710,64 @@
       </c>
       <c r="F17" s="16"/>
       <c r="G17" s="15">
-        <f>SUM(G5:G16)</f>
+        <f t="shared" ref="G17:T17" si="3">SUM(G5:G16)</f>
         <v>0</v>
       </c>
       <c r="H17" s="15">
-        <f>SUM(H5:H16)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I17" s="15">
-        <f>SUM(I5:I16)</f>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="J17" s="15">
-        <f>SUM(J5:J16)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K17" s="15">
-        <f>SUM(K5:K16)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L17" s="15">
-        <f>SUM(L5:L16)</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="M17" s="15">
-        <f>SUM(M5:M16)</f>
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="N17" s="15">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N17" s="15">
-        <f>SUM(N5:N16)</f>
+      <c r="O17" s="15">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="O17" s="15">
-        <f>SUM(O5:O16)</f>
+      <c r="P17" s="15">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="P17" s="15">
-        <f>SUM(P5:P16)</f>
+      <c r="Q17" s="15">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="Q17" s="15">
-        <f>SUM(Q5:Q16)</f>
+      <c r="R17" s="15">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="R17" s="15">
-        <f>SUM(R5:R16)</f>
+      <c r="S17" s="15">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="S17" s="15">
-        <f>SUM(S5:S16)</f>
-        <v>0</v>
-      </c>
       <c r="T17" s="15">
-        <f>SUM(T5:T16)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="U17" s="15">
         <f t="shared" si="0"/>
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
@@ -2851,60 +2853,60 @@
         <v>38</v>
       </c>
       <c r="G19" s="15">
-        <f>F19-SUM(G5:G16)</f>
+        <f t="shared" ref="G19:T19" si="4">F19-SUM(G5:G16)</f>
         <v>38</v>
       </c>
       <c r="H19" s="15">
-        <f>G19-SUM(H5:H16)</f>
+        <f t="shared" si="4"/>
         <v>38</v>
       </c>
       <c r="I19" s="15">
-        <f>H19-SUM(I5:I16)</f>
+        <f t="shared" si="4"/>
         <v>32</v>
       </c>
       <c r="J19" s="15">
-        <f>I19-SUM(J5:J16)</f>
+        <f t="shared" si="4"/>
         <v>32</v>
       </c>
       <c r="K19" s="15">
-        <f>J19-SUM(K5:K16)</f>
+        <f t="shared" si="4"/>
         <v>32</v>
       </c>
       <c r="L19" s="15">
-        <f>K19-SUM(L5:L16)</f>
+        <f t="shared" si="4"/>
         <v>29</v>
       </c>
       <c r="M19" s="15">
-        <f>L19-SUM(M5:M16)</f>
-        <v>29</v>
+        <f t="shared" si="4"/>
+        <v>26</v>
       </c>
       <c r="N19" s="15">
-        <f>M19-SUM(N5:N16)</f>
-        <v>29</v>
+        <f t="shared" si="4"/>
+        <v>26</v>
       </c>
       <c r="O19" s="15">
-        <f>N19-SUM(O5:O16)</f>
-        <v>29</v>
+        <f t="shared" si="4"/>
+        <v>26</v>
       </c>
       <c r="P19" s="15">
-        <f>O19-SUM(P5:P16)</f>
-        <v>29</v>
+        <f t="shared" si="4"/>
+        <v>26</v>
       </c>
       <c r="Q19" s="15">
-        <f>P19-SUM(Q5:Q16)</f>
-        <v>29</v>
+        <f t="shared" si="4"/>
+        <v>26</v>
       </c>
       <c r="R19" s="15">
-        <f>Q19-SUM(R5:R16)</f>
-        <v>29</v>
+        <f t="shared" si="4"/>
+        <v>26</v>
       </c>
       <c r="S19" s="15">
-        <f>R19-SUM(S5:S16)</f>
-        <v>29</v>
+        <f t="shared" si="4"/>
+        <v>26</v>
       </c>
       <c r="T19" s="15">
-        <f>S19-SUM(T5:T16)</f>
-        <v>29</v>
+        <f t="shared" si="4"/>
+        <v>26</v>
       </c>
       <c r="U19" s="17"/>
     </row>

</xml_diff>

<commit_message>
Scrum daily standup, day 8
</commit_message>
<xml_diff>
--- a/Sprint_info/Sprint2.xlsx
+++ b/Sprint_info/Sprint2.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="57">
   <si>
     <t>Name</t>
   </si>
@@ -848,25 +848,25 @@
                   <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>26</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>26</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>26</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>26</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>26</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>26</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>26</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2173,7 +2173,7 @@
   <dimension ref="A1:U25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2358,7 +2358,9 @@
       <c r="C7" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="D7" s="15"/>
+      <c r="D7" s="15" t="s">
+        <v>3</v>
+      </c>
       <c r="E7" s="15">
         <v>1</v>
       </c>
@@ -2428,12 +2430,14 @@
       <c r="C9" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="15"/>
+      <c r="D9" s="15" t="s">
+        <v>9</v>
+      </c>
       <c r="E9" s="15">
         <v>3</v>
       </c>
       <c r="F9" s="15" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G9" s="15"/>
       <c r="H9" s="15"/>
@@ -2442,7 +2446,9 @@
       <c r="K9" s="15"/>
       <c r="L9" s="15"/>
       <c r="M9" s="15"/>
-      <c r="N9" s="15"/>
+      <c r="N9" s="15">
+        <v>3</v>
+      </c>
       <c r="O9" s="15"/>
       <c r="P9" s="15"/>
       <c r="Q9" s="15"/>
@@ -2451,7 +2457,7 @@
       <c r="T9" s="15"/>
       <c r="U9" s="15">
         <f t="shared" ref="U9:U10" si="1">E9-SUM(G9:T9)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2467,7 +2473,7 @@
         <v>3</v>
       </c>
       <c r="F10" s="15" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G10" s="15"/>
       <c r="H10" s="15"/>
@@ -2476,7 +2482,9 @@
       <c r="K10" s="15"/>
       <c r="L10" s="15"/>
       <c r="M10" s="15"/>
-      <c r="N10" s="15"/>
+      <c r="N10" s="15">
+        <v>3</v>
+      </c>
       <c r="O10" s="15"/>
       <c r="P10" s="15"/>
       <c r="Q10" s="15"/>
@@ -2485,7 +2493,7 @@
       <c r="T10" s="15"/>
       <c r="U10" s="15">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2505,7 +2513,7 @@
         <v>5</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G11" s="15"/>
       <c r="H11" s="15"/>
@@ -2518,7 +2526,9 @@
       <c r="M11" s="15">
         <v>3</v>
       </c>
-      <c r="N11" s="15"/>
+      <c r="N11" s="15">
+        <v>1</v>
+      </c>
       <c r="O11" s="15"/>
       <c r="P11" s="15"/>
       <c r="Q11" s="15"/>
@@ -2527,7 +2537,7 @@
       <c r="T11" s="15"/>
       <c r="U11" s="15">
         <f>E11-SUM(G11:T11)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2543,7 +2553,7 @@
         <v>5</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G12" s="15"/>
       <c r="H12" s="15"/>
@@ -2570,12 +2580,14 @@
       <c r="C13" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="D13" s="15"/>
+      <c r="D13" s="15" t="s">
+        <v>6</v>
+      </c>
       <c r="E13" s="15">
         <v>5</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G13" s="15"/>
       <c r="H13" s="15"/>
@@ -2609,7 +2621,7 @@
         <v>1</v>
       </c>
       <c r="F14" s="15" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G14" s="15"/>
       <c r="H14" s="15"/>
@@ -2618,7 +2630,9 @@
       <c r="K14" s="15"/>
       <c r="L14" s="15"/>
       <c r="M14" s="15"/>
-      <c r="N14" s="15"/>
+      <c r="N14" s="15">
+        <v>1</v>
+      </c>
       <c r="O14" s="15"/>
       <c r="P14" s="15"/>
       <c r="Q14" s="15"/>
@@ -2627,7 +2641,7 @@
       <c r="T14" s="15"/>
       <c r="U14" s="15">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2636,12 +2650,14 @@
       <c r="C15" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="D15" s="15"/>
+      <c r="D15" s="15" t="s">
+        <v>9</v>
+      </c>
       <c r="E15" s="15">
         <v>1</v>
       </c>
       <c r="F15" s="15" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G15" s="15"/>
       <c r="H15" s="15"/>
@@ -2668,12 +2684,14 @@
       <c r="C16" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="D16" s="15"/>
+      <c r="D16" s="15" t="s">
+        <v>6</v>
+      </c>
       <c r="E16" s="15">
         <v>3</v>
       </c>
       <c r="F16" s="15" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G16" s="15"/>
       <c r="H16" s="15"/>
@@ -2682,7 +2700,9 @@
       <c r="K16" s="15"/>
       <c r="L16" s="15"/>
       <c r="M16" s="15"/>
-      <c r="N16" s="15"/>
+      <c r="N16" s="15">
+        <v>3</v>
+      </c>
       <c r="O16" s="15"/>
       <c r="P16" s="15"/>
       <c r="Q16" s="15"/>
@@ -2691,7 +2711,7 @@
       <c r="T16" s="15"/>
       <c r="U16" s="15">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
@@ -2739,7 +2759,7 @@
       </c>
       <c r="N17" s="15">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="O17" s="15">
         <f t="shared" si="3"/>
@@ -2767,7 +2787,7 @@
       </c>
       <c r="U17" s="15">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
@@ -2882,31 +2902,31 @@
       </c>
       <c r="N19" s="15">
         <f t="shared" si="4"/>
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="O19" s="15">
         <f t="shared" si="4"/>
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="P19" s="15">
         <f t="shared" si="4"/>
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="Q19" s="15">
         <f t="shared" si="4"/>
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="R19" s="15">
         <f t="shared" si="4"/>
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="S19" s="15">
         <f t="shared" si="4"/>
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="T19" s="15">
         <f t="shared" si="4"/>
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="U19" s="17"/>
     </row>

</xml_diff>

<commit_message>
Scrum daily standup, day 9
</commit_message>
<xml_diff>
--- a/Sprint_info/Sprint2.xlsx
+++ b/Sprint_info/Sprint2.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="56">
   <si>
     <t>Name</t>
   </si>
@@ -185,9 +185,6 @@
   </si>
   <si>
     <t>Implement adding new track to timeline</t>
-  </si>
-  <si>
-    <t>To do</t>
   </si>
   <si>
     <t>In progress</t>
@@ -851,22 +848,22 @@
                   <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>15</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>15</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>15</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>15</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>15</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>15</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2173,7 +2170,7 @@
   <dimension ref="A1:U25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2292,7 +2289,7 @@
         <v>3</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G5" s="15"/>
       <c r="H5" s="15"/>
@@ -2330,7 +2327,7 @@
         <v>5</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G6" s="15"/>
       <c r="H6" s="15"/>
@@ -2365,7 +2362,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G7" s="15"/>
       <c r="H7" s="15"/>
@@ -2375,7 +2372,9 @@
       <c r="L7" s="15"/>
       <c r="M7" s="15"/>
       <c r="N7" s="15"/>
-      <c r="O7" s="15"/>
+      <c r="O7" s="15">
+        <v>1</v>
+      </c>
       <c r="P7" s="15"/>
       <c r="Q7" s="15"/>
       <c r="R7" s="15"/>
@@ -2383,7 +2382,7 @@
       <c r="T7" s="15"/>
       <c r="U7" s="15">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
@@ -2394,7 +2393,7 @@
         <v>8</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D8" s="15" t="s">
         <v>3</v>
@@ -2413,7 +2412,9 @@
       <c r="L8" s="15"/>
       <c r="M8" s="15"/>
       <c r="N8" s="15"/>
-      <c r="O8" s="15"/>
+      <c r="O8" s="15">
+        <v>3</v>
+      </c>
       <c r="P8" s="15"/>
       <c r="Q8" s="15"/>
       <c r="R8" s="15"/>
@@ -2421,7 +2422,7 @@
       <c r="T8" s="15"/>
       <c r="U8" s="15">
         <f>E8-SUM(G8:T8)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
@@ -2437,7 +2438,7 @@
         <v>3</v>
       </c>
       <c r="F9" s="15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G9" s="15"/>
       <c r="H9" s="15"/>
@@ -2473,7 +2474,7 @@
         <v>3</v>
       </c>
       <c r="F10" s="15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G10" s="15"/>
       <c r="H10" s="15"/>
@@ -2513,7 +2514,7 @@
         <v>5</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G11" s="15"/>
       <c r="H11" s="15"/>
@@ -2553,7 +2554,7 @@
         <v>5</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G12" s="15"/>
       <c r="H12" s="15"/>
@@ -2563,7 +2564,9 @@
       <c r="L12" s="15"/>
       <c r="M12" s="15"/>
       <c r="N12" s="15"/>
-      <c r="O12" s="15"/>
+      <c r="O12" s="15">
+        <v>2</v>
+      </c>
       <c r="P12" s="15"/>
       <c r="Q12" s="15"/>
       <c r="R12" s="15"/>
@@ -2571,7 +2574,7 @@
       <c r="T12" s="15"/>
       <c r="U12" s="15">
         <f>E12-SUM(G12:T12)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2587,7 +2590,7 @@
         <v>5</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G13" s="15"/>
       <c r="H13" s="15"/>
@@ -2597,7 +2600,9 @@
       <c r="L13" s="15"/>
       <c r="M13" s="15"/>
       <c r="N13" s="15"/>
-      <c r="O13" s="15"/>
+      <c r="O13" s="15">
+        <v>1</v>
+      </c>
       <c r="P13" s="15"/>
       <c r="Q13" s="15"/>
       <c r="R13" s="15"/>
@@ -2605,7 +2610,7 @@
       <c r="T13" s="15"/>
       <c r="U13" s="15">
         <f t="shared" ref="U13:U16" si="2">E13-SUM(G13:T13)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2621,7 +2626,7 @@
         <v>1</v>
       </c>
       <c r="F14" s="15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G14" s="15"/>
       <c r="H14" s="15"/>
@@ -2648,7 +2653,7 @@
       <c r="A15" s="25"/>
       <c r="B15" s="25"/>
       <c r="C15" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D15" s="15" t="s">
         <v>9</v>
@@ -2657,7 +2662,7 @@
         <v>1</v>
       </c>
       <c r="F15" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G15" s="15"/>
       <c r="H15" s="15"/>
@@ -2691,7 +2696,7 @@
         <v>3</v>
       </c>
       <c r="F16" s="15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G16" s="15"/>
       <c r="H16" s="15"/>
@@ -2763,7 +2768,7 @@
       </c>
       <c r="O17" s="15">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="P17" s="15">
         <f t="shared" si="3"/>
@@ -2787,7 +2792,7 @@
       </c>
       <c r="U17" s="15">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
@@ -2906,27 +2911,27 @@
       </c>
       <c r="O19" s="15">
         <f t="shared" si="4"/>
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="P19" s="15">
         <f t="shared" si="4"/>
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="Q19" s="15">
         <f t="shared" si="4"/>
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="R19" s="15">
         <f t="shared" si="4"/>
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="S19" s="15">
         <f t="shared" si="4"/>
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="T19" s="15">
         <f t="shared" si="4"/>
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="U19" s="17"/>
     </row>
@@ -3016,8 +3021,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="Q19" sqref="Q19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>